<commit_message>
Adição dos exercicios de lista
</commit_message>
<xml_diff>
--- a/ExerciciosTeams2/TestesDMesa.xlsx
+++ b/ExerciciosTeams2/TestesDMesa.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caueh\Desktop\ExerciciosLP 2\ExerciciosTeams2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fatecspgov-my.sharepoint.com/personal/caue_silva10_fatec_sp_gov_br/Documents/desktopnotebook/Branch/DevMinds/LP1/ExerciciosTeams2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306B7B14-D44F-47DF-A9EE-980DA15C593F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{306B7B14-D44F-47DF-A9EE-980DA15C593F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AD626BE-95A9-460C-B255-DE28433DF0D4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B5CB70CB-0A17-496E-9952-DEDA4394463D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{B5CB70CB-0A17-496E-9952-DEDA4394463D}"/>
   </bookViews>
   <sheets>
     <sheet name="78" sheetId="3" r:id="rId1"/>
     <sheet name="79" sheetId="4" r:id="rId2"/>
     <sheet name="82" sheetId="1" r:id="rId3"/>
+    <sheet name="80" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -115,9 +116,6 @@
     <t>[20,10,5,90,700,1,40,80,100,null]</t>
   </si>
   <si>
-    <t>{ACHEI}</t>
-  </si>
-  <si>
     <t>[Ana]</t>
   </si>
   <si>
@@ -136,9 +134,6 @@
     <t>Encontrado</t>
   </si>
   <si>
-    <t>Output</t>
-  </si>
-  <si>
     <t>[Caue]</t>
   </si>
   <si>
@@ -233,6 +228,12 @@
   </si>
   <si>
     <t>[10,10,10,10,10,10,10,10,10,10,10,10,2,2,2,2,2,2,2,0]</t>
+  </si>
+  <si>
+    <t>Saida</t>
+  </si>
+  <si>
+    <t>Achei!</t>
   </si>
 </sst>
 </file>
@@ -357,12 +358,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -373,52 +374,7 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -609,13 +565,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="1"/>
         </left>
@@ -629,6 +578,61 @@
           <color theme="1"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -738,9 +742,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -755,28 +756,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C8B37018-B95D-437E-AFF7-461F00634B54}" name="Tabela3" displayName="Tabela3" ref="A1:E15" totalsRowShown="0" dataDxfId="10" dataCellStyle="Normal 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C8B37018-B95D-437E-AFF7-461F00634B54}" name="Tabela3" displayName="Tabela3" ref="A1:E15" totalsRowShown="0" dataDxfId="16" dataCellStyle="Normal 3">
   <autoFilter ref="A1:E15" xr:uid="{C8B37018-B95D-437E-AFF7-461F00634B54}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8B446F64-BA61-4875-A254-5EA9975E72BD}" name="Nome" dataDxfId="15" dataCellStyle="Normal 3"/>
     <tableColumn id="2" xr3:uid="{A750BB89-AF13-4C1E-8B37-094EA54B4978}" name="Input" dataDxfId="14" dataCellStyle="Normal 3"/>
     <tableColumn id="3" xr3:uid="{FA02163F-92B8-4BE5-9596-A452B77EB696}" name="Nome Buscado" dataDxfId="13" dataCellStyle="Normal 3"/>
     <tableColumn id="4" xr3:uid="{44399A37-34B9-44E5-806F-E4208C5E40CE}" name="Encontrado" dataDxfId="12" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" xr3:uid="{D4E3731D-0812-49EA-BF7D-6D0E16ABC2BE}" name="Output" dataDxfId="11" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{D4E3731D-0812-49EA-BF7D-6D0E16ABC2BE}" name="Saida" dataDxfId="11" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C7D67E0C-00F6-4D90-BF4F-07223B5BE1E6}" name="Tabela4" displayName="Tabela4" ref="A1:E9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C7D67E0C-00F6-4D90-BF4F-07223B5BE1E6}" name="Tabela4" displayName="Tabela4" ref="A1:E9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A1:E9" xr:uid="{C7D67E0C-00F6-4D90-BF4F-07223B5BE1E6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{24334E66-F31C-4123-8C01-B5E7AAF3AA37}" name="Notas" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{0ACEEC21-5B71-4025-B194-77F7B6D3AF5B}" name="Entrada" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{39911A0F-9BE6-4E95-8BBD-65A0B0DC2993}" name="Soma" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{47CDD588-14AD-4945-B7A8-B3A815754757}" name="Média" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{224786B1-4802-4E61-AC66-4DB1FB725A27}" name="Qtd. Acima da média" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{24334E66-F31C-4123-8C01-B5E7AAF3AA37}" name="Notas" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{0ACEEC21-5B71-4025-B194-77F7B6D3AF5B}" name="Entrada" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{39911A0F-9BE6-4E95-8BBD-65A0B0DC2993}" name="Soma" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{47CDD588-14AD-4945-B7A8-B3A815754757}" name="Média" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{224786B1-4802-4E61-AC66-4DB1FB725A27}" name="Qtd. Acima da média" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -788,7 +789,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{15220F39-81B2-402C-97AF-5F448126188C}" name="Vetor A"/>
     <tableColumn id="2" xr3:uid="{30D2D074-355E-40B4-80B2-B88BD793B292}" name="Vetor M"/>
-    <tableColumn id="3" xr3:uid="{64DF0128-708E-426B-8BE6-22C61B6E7A9D}" name="X" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{64DF0128-708E-426B-8BE6-22C61B6E7A9D}" name="X" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1097,37 +1098,37 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="12.5703125" style="6"/>
+    <col min="1" max="1" width="58.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="12.5546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
       <c r="E1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1144,207 +1145,207 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>36</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
         <v>44</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
       <c r="E14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
@@ -1353,10 +1354,10 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1374,125 +1375,125 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="12.5703125" style="5"/>
+    <col min="2" max="2" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="12.5546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>3</v>
@@ -1507,9 +1508,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>3</v>
@@ -1524,9 +1525,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>3</v>
@@ -1557,14 +1558,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="63" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="82.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +1576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1586,7 +1587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1597,7 +1598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1608,7 +1609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1619,7 +1620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1641,7 +1642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1652,7 +1653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1663,7 +1664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1674,7 +1675,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1696,7 +1697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1707,7 +1708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1718,7 +1719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1740,7 +1741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1751,7 +1752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1784,7 +1785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1806,7 +1807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1817,7 +1818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1828,7 +1829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1846,4 +1847,18 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64201BA2-18F0-49A9-93F0-8E302BCA99B8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adição de mais testes de mesa
Adição de mais testes de mesa
</commit_message>
<xml_diff>
--- a/ExerciciosTeams2/TestesDMesa.xlsx
+++ b/ExerciciosTeams2/TestesDMesa.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fatecspgov-my.sharepoint.com/personal/caue_silva10_fatec_sp_gov_br/Documents/desktopnotebook/Branch/DevMinds/LP1/ExerciciosTeams2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{306B7B14-D44F-47DF-A9EE-980DA15C593F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AD626BE-95A9-460C-B255-DE28433DF0D4}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{306B7B14-D44F-47DF-A9EE-980DA15C593F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D3477BA-B412-45DB-B9BF-A0ACE1B5BF7D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{B5CB70CB-0A17-496E-9952-DEDA4394463D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{B5CB70CB-0A17-496E-9952-DEDA4394463D}"/>
   </bookViews>
   <sheets>
     <sheet name="78" sheetId="3" r:id="rId1"/>
     <sheet name="79" sheetId="4" r:id="rId2"/>
-    <sheet name="82" sheetId="1" r:id="rId3"/>
-    <sheet name="80" sheetId="5" r:id="rId4"/>
+    <sheet name="80" sheetId="5" r:id="rId3"/>
+    <sheet name="81" sheetId="6" r:id="rId4"/>
+    <sheet name="82" sheetId="1" r:id="rId5"/>
+    <sheet name="83" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="87">
   <si>
     <t>Vetor A</t>
   </si>
@@ -234,13 +236,79 @@
   </si>
   <si>
     <t>Achei!</t>
+  </si>
+  <si>
+    <t>VetorQ</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0]</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>[1,2,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0]</t>
+  </si>
+  <si>
+    <t>[1,2,3,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0]</t>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t>[1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,0]</t>
+  </si>
+  <si>
+    <t>[19]</t>
+  </si>
+  <si>
+    <t>[1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20]</t>
+  </si>
+  <si>
+    <t>[20]</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>Maior</t>
+  </si>
+  <si>
+    <t>MaiorPosição</t>
+  </si>
+  <si>
+    <t>Menor</t>
+  </si>
+  <si>
+    <t>Menor Posição</t>
+  </si>
+  <si>
+    <t>[0,19,18,17,16,15,14,13,12,11,10,9,8,7,6,5,4,3,2,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,3,2,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,2,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1]</t>
+  </si>
+  <si>
+    <t>Vetor</t>
+  </si>
+  <si>
+    <t>Vetor Inverso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,19 +350,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -352,27 +421,325 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{109A18B3-F127-45CD-B31F-B623C3413930}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{CB1C6405-B261-4A78-AEBA-9DCF8F18AF34}"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -755,41 +1122,83 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C8B37018-B95D-437E-AFF7-461F00634B54}" name="Tabela3" displayName="Tabela3" ref="A1:E15" totalsRowShown="0" dataDxfId="16" dataCellStyle="Normal 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C8B37018-B95D-437E-AFF7-461F00634B54}" name="Tabela3" displayName="Tabela3" ref="A1:E15" totalsRowShown="0" dataDxfId="31" dataCellStyle="Normal 3">
   <autoFilter ref="A1:E15" xr:uid="{C8B37018-B95D-437E-AFF7-461F00634B54}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8B446F64-BA61-4875-A254-5EA9975E72BD}" name="Nome" dataDxfId="15" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" xr3:uid="{A750BB89-AF13-4C1E-8B37-094EA54B4978}" name="Input" dataDxfId="14" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" xr3:uid="{FA02163F-92B8-4BE5-9596-A452B77EB696}" name="Nome Buscado" dataDxfId="13" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" xr3:uid="{44399A37-34B9-44E5-806F-E4208C5E40CE}" name="Encontrado" dataDxfId="12" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" xr3:uid="{D4E3731D-0812-49EA-BF7D-6D0E16ABC2BE}" name="Saida" dataDxfId="11" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{8B446F64-BA61-4875-A254-5EA9975E72BD}" name="Nome" dataDxfId="30" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{A750BB89-AF13-4C1E-8B37-094EA54B4978}" name="Input" dataDxfId="29" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{FA02163F-92B8-4BE5-9596-A452B77EB696}" name="Nome Buscado" dataDxfId="28" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{44399A37-34B9-44E5-806F-E4208C5E40CE}" name="Encontrado" dataDxfId="27" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{D4E3731D-0812-49EA-BF7D-6D0E16ABC2BE}" name="Saida" dataDxfId="26" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C7D67E0C-00F6-4D90-BF4F-07223B5BE1E6}" name="Tabela4" displayName="Tabela4" ref="A1:E9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C7D67E0C-00F6-4D90-BF4F-07223B5BE1E6}" name="Tabela4" displayName="Tabela4" ref="A1:E9" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="A1:E9" xr:uid="{C7D67E0C-00F6-4D90-BF4F-07223B5BE1E6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{24334E66-F31C-4123-8C01-B5E7AAF3AA37}" name="Notas" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{0ACEEC21-5B71-4025-B194-77F7B6D3AF5B}" name="Entrada" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{39911A0F-9BE6-4E95-8BBD-65A0B0DC2993}" name="Soma" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{47CDD588-14AD-4945-B7A8-B3A815754757}" name="Média" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{224786B1-4802-4E61-AC66-4DB1FB725A27}" name="Qtd. Acima da média" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{24334E66-F31C-4123-8C01-B5E7AAF3AA37}" name="Notas" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{0ACEEC21-5B71-4025-B194-77F7B6D3AF5B}" name="Entrada" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{39911A0F-9BE6-4E95-8BBD-65A0B0DC2993}" name="Soma" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{47CDD588-14AD-4945-B7A8-B3A815754757}" name="Média" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{224786B1-4802-4E61-AC66-4DB1FB725A27}" name="Qtd. Acima da média" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D644668A-FFF4-48CF-B65E-2A52D7B60767}" name="Tabela2" displayName="Tabela2" ref="A1:D9" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A1:D9" xr:uid="{D644668A-FFF4-48CF-B65E-2A52D7B60767}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E2504712-02E4-492C-B291-5CB954B71207}" name="VetorQ" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{78751D49-CE0E-4E22-BFC1-B8701A0953D9}" name="Numero" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{CE034142-E2DF-4198-9734-7B33E803AE63}" name="Maior" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{8973D997-BF07-44E1-8DEB-0D9C9E0D0FFC}" name="MaiorPosição" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8F4593D5-739E-4682-961C-AF8D3CE48AFF}" name="Tabela5" displayName="Tabela5" ref="A1:D9" totalsRowShown="0" headerRowDxfId="9" headerRowCellStyle="Normal 2">
+  <autoFilter ref="A1:D9" xr:uid="{8F4593D5-739E-4682-961C-AF8D3CE48AFF}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{F8D9C8B8-FED5-4CA4-9B60-A441B7184481}" name="VetorQ" dataDxfId="8" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{85FB58D7-491C-4F54-A806-0ABC3B971EFC}" name="Numero" dataDxfId="7" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{801B9E99-07F9-412A-9237-0F1BFEA45679}" name="Menor" dataDxfId="6" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" xr3:uid="{51CD40C1-E81B-4818-96C5-60B8AD2FE90D}" name="Menor Posição" dataDxfId="5" dataCellStyle="Normal 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DBC57251-AABE-4511-AD3C-72B31BE39FF8}" name="Tabela1" displayName="Tabela1" ref="A1:C25" totalsRowShown="0">
   <autoFilter ref="A1:C25" xr:uid="{DBC57251-AABE-4511-AD3C-72B31BE39FF8}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{15220F39-81B2-402C-97AF-5F448126188C}" name="Vetor A"/>
     <tableColumn id="2" xr3:uid="{30D2D074-355E-40B4-80B2-B88BD793B292}" name="Vetor M"/>
-    <tableColumn id="3" xr3:uid="{64DF0128-708E-426B-8BE6-22C61B6E7A9D}" name="X" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{64DF0128-708E-426B-8BE6-22C61B6E7A9D}" name="X" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F045EEF6-EDFC-4B61-84D4-D4A2B5F132A7}" name="Tabela6" displayName="Tabela6" ref="A1:C8" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowCellStyle="Normal 3" dataCellStyle="Normal 3">
+  <autoFilter ref="A1:C8" xr:uid="{F045EEF6-EDFC-4B61-84D4-D4A2B5F132A7}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{76F7F040-D5A5-4D13-A773-495C387CA328}" name="Vetor" dataDxfId="4" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{70A7FBB2-1862-4076-BF06-2C95DA8A95EB}" name="Vetor Inverso" dataDxfId="3" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{1253FEC7-19FD-4932-B3E3-6D694168B967}" name="Input" dataDxfId="2" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1101,17 +1510,17 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="12.5546875" style="6"/>
+    <col min="1" max="1" width="58.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="12.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1128,7 +1537,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1145,7 +1554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1156,11 +1565,11 @@
       <c r="D3"/>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C4" t="s">
@@ -1173,7 +1582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1190,7 +1599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1207,7 +1616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1224,7 +1633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1241,7 +1650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1258,7 +1667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -1275,7 +1684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1292,7 +1701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1309,7 +1718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -1326,7 +1735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1343,7 +1752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1375,170 +1784,170 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="12.5546875" style="5"/>
+    <col min="1" max="1" width="47" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="12.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="10">
+      <c r="B7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="9">
         <v>128</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="D7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="10">
+      <c r="B8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9">
         <v>128</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>6.8</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="E8" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="10">
+      <c r="B9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9">
         <v>128</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>6.8</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>12</v>
       </c>
     </row>
@@ -1551,21 +1960,325 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64201BA2-18F0-49A9-93F0-8E302BCA99B8}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E620BD6-B07D-4951-952D-CA4593BEE27B}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="12.5703125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF3AFF3-9DCB-41F4-A5B8-94231E8AEE6E}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63" customWidth="1"/>
-    <col min="2" max="2" width="82.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1576,7 +2289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1587,7 +2300,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1598,7 +2311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1609,7 +2322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1620,7 +2333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1631,7 +2344,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1642,7 +2355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1653,7 +2366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1664,7 +2377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1675,7 +2388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1686,7 +2399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1697,7 +2410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1708,7 +2421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1719,7 +2432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1730,7 +2443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1741,7 +2454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1752,7 +2465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1763,7 +2476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1774,7 +2487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1785,7 +2498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1796,7 +2509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1807,7 +2520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1818,7 +2531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1829,11 +2542,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="1">
@@ -1849,16 +2562,116 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64201BA2-18F0-49A9-93F0-8E302BCA99B8}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3F8F37-A914-4301-B8B8-FA653EE2DD25}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J16"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="38.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="12.5703125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>